<commit_message>
Resoluçõa da Quarta Questão
</commit_message>
<xml_diff>
--- a/Dados/Questao3.xlsx
+++ b/Dados/Questao3.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edevaldogaudencio/Documents/Pessoal/Educação/FGV/Mestrado Profissional em Economia/2_2020/Estatística/Listas de Exercícios/Lista 1/dados/MestradoEstatisticaLista1/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F3D6A2-C1B7-E446-8494-218F91506E50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC0EAAF-0382-274F-90B0-BFA385B17AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="1960" windowWidth="26680" windowHeight="15540" xr2:uid="{A02B67FA-B643-B746-B20D-453CE0227461}"/>
   </bookViews>
   <sheets>
     <sheet name="tx cresc pop" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -382,7 +382,7 @@
   <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>